<commit_message>
Initial workflow framework, example data extraction
Begin adding in project workflow pipeline, from data
extraction up to building figures, tables and final
documents.  Create example data extraction of raw
subject trials into tidy csv file for better data
analysis.

Add in some raw data files to repository for testing.
These will eventually be removed when want to generated/run
real experiments.
</commit_message>
<xml_diff>
--- a/exp/stroop-replication-trialtypes.xlsx
+++ b/exp/stroop-replication-trialtypes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
   <si>
     <t xml:space="preserve">text</t>
   </si>
@@ -28,7 +28,7 @@
     <t xml:space="preserve">letterColor</t>
   </si>
   <si>
-    <t xml:space="preserve">corrAns</t>
+    <t xml:space="preserve">correctAnswer</t>
   </si>
   <si>
     <t xml:space="preserve">congruent</t>
@@ -40,16 +40,13 @@
     <t xml:space="preserve">z</t>
   </si>
   <si>
-    <t xml:space="preserve">cong</t>
-  </si>
-  <si>
     <t xml:space="preserve">green</t>
   </si>
   <si>
     <t xml:space="preserve">m</t>
   </si>
   <si>
-    <t xml:space="preserve">incong</t>
+    <t xml:space="preserve">incongruent</t>
   </si>
 </sst>
 </file>
@@ -153,7 +150,7 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -183,7 +180,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -191,18 +188,18 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -211,21 +208,21 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Update experiment trial workflow
Update experiment trial workflow to what should be about the final
version we need.  This stroop replicatione experiment does the following

- Prompts and records participant number, session number and posture condition
- Runs 1 block of 36 practice trials
- Gives feedback in form of sound and reaction time result for practice
- Has a limit of 1.5 seconds to respond on trials
- Runs 2 blocks of 36 trials for real data
- Give sound feedback but no other information on the real trials.

It is assumed that the experimenter will run subject in 1 posture first.
Then reposition subject for new posture and run a second time with the
same participant id.  Thus we will end up with 2 separate files for
each participant, containing the sitting and standing posture data
respectively.
</commit_message>
<xml_diff>
--- a/exp/stroop-replication-trialtypes.xlsx
+++ b/exp/stroop-replication-trialtypes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="12">
   <si>
     <t xml:space="preserve">text</t>
   </si>
@@ -34,16 +34,25 @@
     <t xml:space="preserve">congruent</t>
   </si>
   <si>
+    <t xml:space="preserve">XXX</t>
+  </si>
+  <si>
     <t xml:space="preserve">red</t>
   </si>
   <si>
     <t xml:space="preserve">z</t>
   </si>
   <si>
+    <t xml:space="preserve">neutral</t>
+  </si>
+  <si>
     <t xml:space="preserve">green</t>
   </si>
   <si>
     <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XXXXX</t>
   </si>
   <si>
     <t xml:space="preserve">incongruent</t>
@@ -150,7 +159,7 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -174,13 +183,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -188,40 +197,488 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor experiment flow, single executable and cocunterbalancing
Refactored psychopy experiment file to flow as a single experiment
that runs both sitting and standing conditions for a subject.
This refactoring performs counterbalancing of two separate conditions.
Subjects can start the experiment either standing or sitting, and then
move to the other posture (within subject).  Also subjects will either
perform the experiment with red mapped to left button and green to
right button, or reversed.  Subjects do both postures but will do all
trials with a single key mapping (between subjects).

We map subject id to counterbalancing condition.

1000-1999: initial standing / red-left green-right
2000-2999: initial standing / green-left red-right
3000-3999: initial sitting  / red-left green-right
4000-4999: initial sitting  / green-left red-right
</commit_message>
<xml_diff>
--- a/exp/stroop-replication-trialtypes.xlsx
+++ b/exp/stroop-replication-trialtypes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="9">
   <si>
     <t xml:space="preserve">text</t>
   </si>
@@ -28,9 +28,6 @@
     <t xml:space="preserve">letterColor</t>
   </si>
   <si>
-    <t xml:space="preserve">correctAnswer</t>
-  </si>
-  <si>
     <t xml:space="preserve">congruent</t>
   </si>
   <si>
@@ -40,16 +37,10 @@
     <t xml:space="preserve">red</t>
   </si>
   <si>
-    <t xml:space="preserve">z</t>
-  </si>
-  <si>
     <t xml:space="preserve">neutral</t>
   </si>
   <si>
     <t xml:space="preserve">green</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m</t>
   </si>
   <si>
     <t xml:space="preserve">XXXXX</t>
@@ -156,15 +147,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1048576"/>
+  <dimension ref="A1:AMJ37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.08"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -174,528 +168,404 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>